<commit_message>
Added Capacitance vs Reverse Voltage Measurements for SMV1249
Added formatting to both  varactor measurement excel sheets as well. Measurements were taken by unsoldering BBY40 from build test fixture and soldering in SMV1249 in its place.
</commit_message>
<xml_diff>
--- a/Measurements/Capacitance/bby40Measurement.xlsx
+++ b/Measurements/Capacitance/bby40Measurement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\GitHub\Capstone_Rohde-Schwarz_Team13\Measurements\Capacitance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7384F532-E73B-4911-8894-2CD5342F3DB4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB245FB1-FFC1-4221-AC36-416839A88AAB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="-120" windowWidth="37590" windowHeight="16440" xr2:uid="{58422E9B-39CD-4184-8B40-DBDFB5000FDB}"/>
   </bookViews>
@@ -31,20 +31,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Vr</t>
   </si>
   <si>
     <t>Capacitance</t>
   </si>
+  <si>
+    <t>BBY40 Capacitance Vs. Reverse Voltage Measurements</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -72,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -112,11 +125,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -126,13 +138,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>BBY40 Capacitance (pF) Vs.</a:t>
+              <a:t>BBY40 Capacitance Vs. Reverse Voltage</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Reverse Voltage (V)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -149,11 +156,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -186,29 +192,99 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$12</c:f>
@@ -301,8 +377,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -322,9 +399,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -332,6 +410,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Reverse Voltage (Volts)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -340,9 +471,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -356,9 +486,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -384,9 +513,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -394,6 +524,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Capacitance (pF)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -402,9 +585,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -418,9 +600,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -449,11 +630,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -521,211 +705,35 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -736,78 +744,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -815,58 +752,337 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
           </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:hiLoLine>
   <cs:leaderLine>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -878,27 +1094,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -906,9 +1121,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -918,14 +1132,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -937,12 +1150,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -951,14 +1163,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -967,9 +1180,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -979,17 +1191,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1001,37 +1214,30 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1040,16 +1246,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>366712</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>61912</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1385,10 +1591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B79AFFB-A1D5-47A2-BB48-089FF15FF6A5}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,23 +1602,27 @@
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>67.38</v>
       </c>
+      <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.57199999999999995</v>
       </c>
@@ -1420,7 +1630,7 @@
         <v>53.74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.131</v>
       </c>
@@ -1428,7 +1638,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.595</v>
       </c>
@@ -1436,7 +1646,7 @@
         <v>39.01</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2.0499999999999998</v>
       </c>
@@ -1444,7 +1654,7 @@
         <v>35.1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.59</v>
       </c>
@@ -1452,7 +1662,7 @@
         <v>31.56</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.04</v>
       </c>
@@ -1460,7 +1670,7 @@
         <v>29.24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3.58</v>
       </c>
@@ -1468,7 +1678,7 @@
         <v>26.74</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4.08</v>
       </c>
@@ -1476,7 +1686,7 @@
         <v>24.73</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.59</v>
       </c>
@@ -1484,7 +1694,7 @@
         <v>22.89</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5.01</v>
       </c>

</xml_diff>

<commit_message>
changed scale for model import. idea abandoned
</commit_message>
<xml_diff>
--- a/Measurements/Capacitance/bby40Measurement.xlsx
+++ b/Measurements/Capacitance/bby40Measurement.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\GitHub\Capstone_Rohde-Schwarz_Team13\Measurements\Capacitance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{128D5262-B4E9-464F-9EBD-45A35317CDA8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2CEAC7-B699-4F74-A7B2-AFC06EF9D8FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="-120" windowWidth="37590" windowHeight="16440" xr2:uid="{58422E9B-39CD-4184-8B40-DBDFB5000FDB}"/>
+    <workbookView xWindow="38280" yWindow="-6810" windowWidth="16440" windowHeight="28440" xr2:uid="{58422E9B-39CD-4184-8B40-DBDFB5000FDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -85,9 +84,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -332,40 +332,40 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>67.38</c:v>
+                  <c:v>6.7380000000000004E-11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.74</c:v>
+                  <c:v>5.374E-11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44.1</c:v>
+                  <c:v>4.4100000000000002E-11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.01</c:v>
+                  <c:v>3.9010000000000003E-11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.1</c:v>
+                  <c:v>3.51E-11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.56</c:v>
+                  <c:v>3.1559999999999999E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.24</c:v>
+                  <c:v>2.9240000000000001E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26.74</c:v>
+                  <c:v>2.674E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24.73</c:v>
+                  <c:v>2.4730000000000001E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.89</c:v>
+                  <c:v>2.2890000000000001E-11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.56</c:v>
+                  <c:v>2.1560000000000001E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -578,7 +578,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1594,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B79AFFB-A1D5-47A2-BB48-089FF15FF6A5}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,8 +1618,8 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>67.38</v>
+      <c r="B2" s="2">
+        <v>6.7380000000000004E-11</v>
       </c>
       <c r="J2" s="1"/>
     </row>
@@ -1627,87 +1627,88 @@
       <c r="A3">
         <v>0.57199999999999995</v>
       </c>
-      <c r="B3">
-        <v>53.74</v>
+      <c r="B3" s="2">
+        <v>5.374E-11</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.131</v>
       </c>
-      <c r="B4">
-        <v>44.1</v>
+      <c r="B4" s="2">
+        <v>4.4100000000000002E-11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.595</v>
       </c>
-      <c r="B5">
-        <v>39.01</v>
+      <c r="B5" s="2">
+        <v>3.9010000000000003E-11</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2.0499999999999998</v>
       </c>
-      <c r="B6">
-        <v>35.1</v>
+      <c r="B6" s="2">
+        <v>3.51E-11</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.59</v>
       </c>
-      <c r="B7">
-        <v>31.56</v>
+      <c r="B7" s="2">
+        <v>3.1559999999999999E-11</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.04</v>
       </c>
-      <c r="B8">
-        <v>29.24</v>
+      <c r="B8" s="2">
+        <v>2.9240000000000001E-11</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3.58</v>
       </c>
-      <c r="B9">
-        <v>26.74</v>
+      <c r="B9" s="2">
+        <v>2.674E-11</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4.08</v>
       </c>
-      <c r="B10">
-        <v>24.73</v>
+      <c r="B10" s="2">
+        <v>2.4730000000000001E-11</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.59</v>
       </c>
-      <c r="B11">
-        <v>22.89</v>
+      <c r="B11" s="2">
+        <v>2.2890000000000001E-11</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5.01</v>
       </c>
-      <c r="B12">
-        <v>21.56</v>
+      <c r="B12" s="2">
+        <v>2.1560000000000001E-11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>